<commit_message>
Add comprehensive payroll and payment management system
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ShiftGuard_Complete_System/Excel_Files/ShiftGuard_System.xlsx
+++ b/ShiftGuard_Complete_System/Excel_Files/ShiftGuard_System.xlsx
@@ -10,8 +10,10 @@
     <sheet name="BiometricData" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Calculations" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Dashboard" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ControlPanel" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Payroll" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="PaymentSummary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ControlPanel" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="15">
+  <fonts count="22">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,8 +96,45 @@
       <b val="1"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -132,8 +171,14 @@
         <bgColor rgb="00C00000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4B084"/>
+        <bgColor rgb="00F4B084"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -153,11 +198,39 @@
       <top style="thick"/>
       <bottom style="thick"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -218,6 +291,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -4455,7 +4552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4474,10 +4571,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
@@ -4515,10 +4609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-    </row>
+    <row r="7"/>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
@@ -4546,10 +4637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-    </row>
+    <row r="11"/>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
@@ -4591,10 +4679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-    </row>
+    <row r="16"/>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
@@ -4630,6 +4715,170 @@
       </c>
       <c r="B20" s="6" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="24" t="inlineStr">
+        <is>
+          <t>Payment Configuration</t>
+        </is>
+      </c>
+      <c r="B22" s="24" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="25" t="inlineStr">
+        <is>
+          <t>Hourly Rate (Base)</t>
+        </is>
+      </c>
+      <c r="B23" s="25" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="25" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="B24" s="25" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="25" t="inlineStr">
+        <is>
+          <t>Overtime Multiplier</t>
+        </is>
+      </c>
+      <c r="B25" s="25" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="25" t="inlineStr">
+        <is>
+          <t>Night Shift Allowance %</t>
+        </is>
+      </c>
+      <c r="B26" s="25" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="25" t="inlineStr">
+        <is>
+          <t>Weekend Allowance %</t>
+        </is>
+      </c>
+      <c r="B27" s="25" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="24" t="inlineStr">
+        <is>
+          <t>Deductions &amp; Taxes</t>
+        </is>
+      </c>
+      <c r="B29" s="24" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="25" t="inlineStr">
+        <is>
+          <t>Tax Rate %</t>
+        </is>
+      </c>
+      <c r="B30" s="25" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="25" t="inlineStr">
+        <is>
+          <t>Health Insurance</t>
+        </is>
+      </c>
+      <c r="B31" s="25" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="25" t="inlineStr">
+        <is>
+          <t>Pension Contribution %</t>
+        </is>
+      </c>
+      <c r="B32" s="25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="24" t="inlineStr">
+        <is>
+          <t>Payment Periods</t>
+        </is>
+      </c>
+      <c r="B34" s="24" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="25" t="inlineStr">
+        <is>
+          <t>Pay Frequency</t>
+        </is>
+      </c>
+      <c r="B35" s="25" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="25" t="inlineStr">
+        <is>
+          <t>Pay Day</t>
+        </is>
+      </c>
+      <c r="B36" s="25" t="inlineStr">
+        <is>
+          <t>Last working day</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="25" t="inlineStr">
+        <is>
+          <t>Working Days for Full Pay</t>
+        </is>
+      </c>
+      <c r="B37" s="25" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4650,7 +4899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4667,6 +4916,8 @@
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4710,6 +4961,16 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="I1" s="26" t="inlineStr">
+        <is>
+          <t>Break Penalty</t>
+        </is>
+      </c>
+      <c r="J1" s="26" t="inlineStr">
+        <is>
+          <t>Attendance Bonus</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="8">
@@ -4742,6 +5003,14 @@
       </c>
       <c r="H2" s="9">
         <f>IF(G2&lt;&gt;"",IF(G2&lt;Settings!$B$18,"Low Utilization",IF(E2&gt;Settings!$B$20,"Excessive Overtime","Normal")),"")</f>
+        <v/>
+      </c>
+      <c r="I2" s="27">
+        <f>IF(BiometricData!A2&lt;&gt;"",MAX(0,(BiometricData!E2-Settings!$B$9)/60*Settings!$B$22*0.5),"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="27">
+        <f>IF(AND(BiometricData!A2&lt;&gt;"",G2&gt;=100),Settings!$B$22,"")</f>
         <v/>
       </c>
     </row>
@@ -4756,7 +5025,192 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="28" t="inlineStr">
+        <is>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B1" s="28" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="28" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="D1" s="28" t="inlineStr">
+        <is>
+          <t>Regular Hours</t>
+        </is>
+      </c>
+      <c r="E1" s="28" t="inlineStr">
+        <is>
+          <t>Overtime Hours</t>
+        </is>
+      </c>
+      <c r="F1" s="28" t="inlineStr">
+        <is>
+          <t>Night Hours</t>
+        </is>
+      </c>
+      <c r="G1" s="28" t="inlineStr">
+        <is>
+          <t>Base Pay</t>
+        </is>
+      </c>
+      <c r="H1" s="28" t="inlineStr">
+        <is>
+          <t>Overtime Pay</t>
+        </is>
+      </c>
+      <c r="I1" s="28" t="inlineStr">
+        <is>
+          <t>Night Allowance</t>
+        </is>
+      </c>
+      <c r="J1" s="28" t="inlineStr">
+        <is>
+          <t>Weekend Allowance</t>
+        </is>
+      </c>
+      <c r="K1" s="28" t="inlineStr">
+        <is>
+          <t>Gross Pay</t>
+        </is>
+      </c>
+      <c r="L1" s="28" t="inlineStr">
+        <is>
+          <t>Tax Deduction</t>
+        </is>
+      </c>
+      <c r="M1" s="28" t="inlineStr">
+        <is>
+          <t>Health Insurance</t>
+        </is>
+      </c>
+      <c r="N1" s="28" t="inlineStr">
+        <is>
+          <t>Pension Deduction</t>
+        </is>
+      </c>
+      <c r="O1" s="28" t="inlineStr">
+        <is>
+          <t>Total Deductions</t>
+        </is>
+      </c>
+      <c r="P1" s="28" t="inlineStr">
+        <is>
+          <t>Net Pay</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8">
+        <f>BiometricData!A2</f>
+        <v/>
+      </c>
+      <c r="B2" s="8">
+        <f>BiometricData!B2</f>
+        <v/>
+      </c>
+      <c r="C2" s="8">
+        <f>BiometricData!G2</f>
+        <v/>
+      </c>
+      <c r="D2" s="8">
+        <f>MIN(Calculations!C2,Settings!$B$4)</f>
+        <v/>
+      </c>
+      <c r="E2" s="8">
+        <f>Calculations!E2</f>
+        <v/>
+      </c>
+      <c r="F2" s="8">
+        <f>Calculations!F2</f>
+        <v/>
+      </c>
+      <c r="G2" s="27">
+        <f>IF(A2&lt;&gt;"",D2*Settings!$B$22,"")</f>
+        <v/>
+      </c>
+      <c r="H2" s="27">
+        <f>IF(A2&lt;&gt;"",E2*Settings!$B$22*Settings!$B$24,"")</f>
+        <v/>
+      </c>
+      <c r="I2" s="27">
+        <f>IF(A2&lt;&gt;"",F2*Settings!$B$22*Settings!$B$25/100,"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="27">
+        <f>IF(AND(A2&lt;&gt;"",OR(WEEKDAY(B2)=1,WEEKDAY(B2)=7)),D2*Settings!$B$22*Settings!$B$26/100,0)</f>
+        <v/>
+      </c>
+      <c r="K2" s="27">
+        <f>IF(A2&lt;&gt;"",G2+H2+I2+J2,"")</f>
+        <v/>
+      </c>
+      <c r="L2" s="27">
+        <f>IF(A2&lt;&gt;"",K2*Settings!$B$28/100,"")</f>
+        <v/>
+      </c>
+      <c r="M2" s="27">
+        <f>IF(A2&lt;&gt;"",Settings!$B$29,"")</f>
+        <v/>
+      </c>
+      <c r="N2" s="27">
+        <f>IF(A2&lt;&gt;"",K2*Settings!$B$30/100,"")</f>
+        <v/>
+      </c>
+      <c r="O2" s="27">
+        <f>IF(A2&lt;&gt;"",L2+M2+N2,"")</f>
+        <v/>
+      </c>
+      <c r="P2" s="27">
+        <f>IF(A2&lt;&gt;"",K2-O2,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4765,7 +5219,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="25" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
@@ -5069,15 +5523,253 @@
         <v/>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="29" t="inlineStr">
+        <is>
+          <t>PAYMENT &amp; PAYROLL METRICS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="30" t="inlineStr">
+        <is>
+          <t>Total Gross Pay</t>
+        </is>
+      </c>
+      <c r="B23" s="31">
+        <f>SUM(Payroll!K:K)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="30" t="inlineStr">
+        <is>
+          <t>Total Deductions</t>
+        </is>
+      </c>
+      <c r="B24" s="31">
+        <f>SUM(Payroll!O:O)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="30" t="inlineStr">
+        <is>
+          <t>Total Net Pay</t>
+        </is>
+      </c>
+      <c r="B25" s="31">
+        <f>SUM(Payroll!P:P)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="30" t="inlineStr">
+        <is>
+          <t>Average Hourly Rate</t>
+        </is>
+      </c>
+      <c r="B26" s="31">
+        <f>Settings!B22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="30" t="inlineStr">
+        <is>
+          <t>Total Overtime Pay</t>
+        </is>
+      </c>
+      <c r="B27" s="31">
+        <f>SUM(Payroll!H:H)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="30" t="inlineStr">
+        <is>
+          <t>Total Night Allowance</t>
+        </is>
+      </c>
+      <c r="B28" s="31">
+        <f>SUM(Payroll!I:I)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="30" t="inlineStr">
+        <is>
+          <t>Average Net Pay/Employee</t>
+        </is>
+      </c>
+      <c r="B29" s="31">
+        <f>IFERROR(SUM(Payroll!P:P)/COUNTA(Payroll!A:A),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="30" t="inlineStr">
+        <is>
+          <t>Payroll Cost/Hour</t>
+        </is>
+      </c>
+      <c r="B30" s="31">
+        <f>IFERROR(SUM(Payroll!K:K)/SUM(Calculations!C:C),0)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="32" t="inlineStr">
+        <is>
+          <t>Employee Payment Summary Report</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="33" t="inlineStr">
+        <is>
+          <t>Generated: 2025-10-31 13:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="34" t="inlineStr">
+        <is>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B4" s="34" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C4" s="34" t="inlineStr">
+        <is>
+          <t>Total Hours</t>
+        </is>
+      </c>
+      <c r="D4" s="34" t="inlineStr">
+        <is>
+          <t>Regular Hours</t>
+        </is>
+      </c>
+      <c r="E4" s="34" t="inlineStr">
+        <is>
+          <t>Overtime Hours</t>
+        </is>
+      </c>
+      <c r="F4" s="34" t="inlineStr">
+        <is>
+          <t>Gross Pay</t>
+        </is>
+      </c>
+      <c r="G4" s="34" t="inlineStr">
+        <is>
+          <t>Deductions</t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="inlineStr">
+        <is>
+          <t>Net Pay</t>
+        </is>
+      </c>
+      <c r="I4" s="34" t="inlineStr">
+        <is>
+          <t>Avg Rate</t>
+        </is>
+      </c>
+      <c r="J4" s="34" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <f>IFERROR(Payroll!A2,"")</f>
+        <v/>
+      </c>
+      <c r="B5">
+        <f>IFERROR(Payroll!C2,"")</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!D:D)+SUMIF(Payroll!A:A,A5,Payroll!E:E),0)</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!D:D),0)</f>
+        <v/>
+      </c>
+      <c r="E5">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!E:E),0)</f>
+        <v/>
+      </c>
+      <c r="F5" s="35">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!K:K),0)</f>
+        <v/>
+      </c>
+      <c r="G5" s="35">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!O:O),0)</f>
+        <v/>
+      </c>
+      <c r="H5" s="35">
+        <f>IFERROR(SUMIF(Payroll!A:A,A5,Payroll!P:P),0)</f>
+        <v/>
+      </c>
+      <c r="I5" s="35">
+        <f>IFERROR(F5/C5,0)</f>
+        <v/>
+      </c>
+      <c r="J5">
+        <f>IF(E5&gt;Settings!$B$20,"High OT","Normal")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5119,6 +5811,9 @@
           <t>Upload Biometric Data</t>
         </is>
       </c>
+      <c r="C6" s="36" t="n"/>
+      <c r="D6" s="36" t="n"/>
+      <c r="E6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="B7" s="21" t="inlineStr">
@@ -5133,6 +5828,9 @@
           <t>Generate Report</t>
         </is>
       </c>
+      <c r="C9" s="36" t="n"/>
+      <c r="D9" s="36" t="n"/>
+      <c r="E9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="B10" s="21" t="inlineStr">
@@ -5147,6 +5845,9 @@
           <t>Export Data to CSV</t>
         </is>
       </c>
+      <c r="C12" s="36" t="n"/>
+      <c r="D12" s="36" t="n"/>
+      <c r="E12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="B13" s="21" t="inlineStr">
@@ -5161,6 +5862,9 @@
           <t>Refresh Dashboard</t>
         </is>
       </c>
+      <c r="C15" s="36" t="n"/>
+      <c r="D15" s="36" t="n"/>
+      <c r="E15" s="37" t="n"/>
     </row>
     <row r="16">
       <c r="B16" s="21" t="inlineStr">
@@ -5175,6 +5879,9 @@
           <t>Validate Data</t>
         </is>
       </c>
+      <c r="C18" s="36" t="n"/>
+      <c r="D18" s="36" t="n"/>
+      <c r="E18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="B19" s="21" t="inlineStr">
@@ -5189,6 +5896,9 @@
           <t>Refresh All</t>
         </is>
       </c>
+      <c r="C21" s="36" t="n"/>
+      <c r="D21" s="36" t="n"/>
+      <c r="E21" s="37" t="n"/>
     </row>
     <row r="22">
       <c r="B22" s="21" t="inlineStr">

</xml_diff>

<commit_message>
Fix formula references and add comprehensive documentation
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ShiftGuard_Complete_System/Excel_Files/ShiftGuard_System.xlsx
+++ b/ShiftGuard_Complete_System/Excel_Files/ShiftGuard_System.xlsx
@@ -4571,7 +4571,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
@@ -4609,7 +4608,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
@@ -4637,7 +4635,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11"/>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
@@ -4679,7 +4676,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16"/>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
@@ -4785,10 +4781,7 @@
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-    </row>
+    <row r="28"/>
     <row r="29">
       <c r="A29" s="24" t="inlineStr">
         <is>
@@ -4833,10 +4826,7 @@
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr"/>
-    </row>
+    <row r="33"/>
     <row r="34">
       <c r="A34" s="24" t="inlineStr">
         <is>
@@ -5010,7 +5000,7 @@
         <v/>
       </c>
       <c r="J2" s="27">
-        <f>IF(AND(BiometricData!A2&lt;&gt;"",G2&gt;=100),Settings!$B$22,"")</f>
+        <f>IF(AND(BiometricData!A2&lt;&gt;"",G2&gt;=100),Settings!$B$23,"")</f>
         <v/>
       </c>
     </row>
@@ -5159,19 +5149,19 @@
         <v/>
       </c>
       <c r="G2" s="27">
-        <f>IF(A2&lt;&gt;"",D2*Settings!$B$22,"")</f>
+        <f>IF(A2&lt;&gt;"",D2*Settings!$B$23,"")</f>
         <v/>
       </c>
       <c r="H2" s="27">
-        <f>IF(A2&lt;&gt;"",E2*Settings!$B$22*Settings!$B$24,"")</f>
+        <f>IF(A2&lt;&gt;"",E2*Settings!$B$23*Settings!$B$25,"")</f>
         <v/>
       </c>
       <c r="I2" s="27">
-        <f>IF(A2&lt;&gt;"",F2*Settings!$B$22*Settings!$B$25/100,"")</f>
+        <f>IF(A2&lt;&gt;"",F2*Settings!$B$23*Settings!$B$26/100,"")</f>
         <v/>
       </c>
       <c r="J2" s="27">
-        <f>IF(AND(A2&lt;&gt;"",OR(WEEKDAY(B2)=1,WEEKDAY(B2)=7)),D2*Settings!$B$22*Settings!$B$26/100,0)</f>
+        <f>IF(AND(A2&lt;&gt;"",OR(WEEKDAY(B2)=1,WEEKDAY(B2)=7)),D2*Settings!$B$23*Settings!$B$27/100,0)</f>
         <v/>
       </c>
       <c r="K2" s="27">
@@ -5179,15 +5169,15 @@
         <v/>
       </c>
       <c r="L2" s="27">
-        <f>IF(A2&lt;&gt;"",K2*Settings!$B$28/100,"")</f>
+        <f>IF(A2&lt;&gt;"",K2*Settings!$B$30/100,"")</f>
         <v/>
       </c>
       <c r="M2" s="27">
-        <f>IF(A2&lt;&gt;"",Settings!$B$29,"")</f>
+        <f>IF(A2&lt;&gt;"",Settings!$B$31,"")</f>
         <v/>
       </c>
       <c r="N2" s="27">
-        <f>IF(A2&lt;&gt;"",K2*Settings!$B$30/100,"")</f>
+        <f>IF(A2&lt;&gt;"",K2*Settings!$B$32/100,"")</f>
         <v/>
       </c>
       <c r="O2" s="27">

</xml_diff>